<commit_message>
Latest automation code with validations
</commit_message>
<xml_diff>
--- a/CommissionDemoData.xlsx
+++ b/CommissionDemoData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PortalPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Commissions Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>sanrao@calliduscloud.com</t>
-  </si>
-  <si>
-    <t>India987&amp;</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -34,6 +28,129 @@
   </si>
   <si>
     <t>https://biz3-tst.callidusondemand.com/SalesPortal/#!/</t>
+  </si>
+  <si>
+    <t>kikosana@calliduscloud.com</t>
+  </si>
+  <si>
+    <t>Kiran09@@</t>
+  </si>
+  <si>
+    <t>Credit Rule</t>
+  </si>
+  <si>
+    <t>Rule Type</t>
+  </si>
+  <si>
+    <t>Deposit Rule</t>
+  </si>
+  <si>
+    <t>Earning Code</t>
+  </si>
+  <si>
+    <t>Earning Type</t>
+  </si>
+  <si>
+    <t>Fixed Value Type</t>
+  </si>
+  <si>
+    <t>Incentive Rule</t>
+  </si>
+  <si>
+    <t>Measurement Rule</t>
+  </si>
+  <si>
+    <t>Plan Components</t>
+  </si>
+  <si>
+    <t>Plans</t>
+  </si>
+  <si>
+    <t>Position Group</t>
+  </si>
+  <si>
+    <t>Rate Table</t>
+  </si>
+  <si>
+    <t>Rate Table variable</t>
+  </si>
+  <si>
+    <t>Reason Codes</t>
+  </si>
+  <si>
+    <t>Territory Elements</t>
+  </si>
+  <si>
+    <t>Territory Variables</t>
+  </si>
+  <si>
+    <t>Unit Type</t>
+  </si>
+  <si>
+    <t>CR Territory Booking</t>
+  </si>
+  <si>
+    <t>Bonus123</t>
+  </si>
+  <si>
+    <t>DR Base Commissions Flat Rate MTD</t>
+  </si>
+  <si>
+    <t>commission</t>
+  </si>
+  <si>
+    <t>Event Type</t>
+  </si>
+  <si>
+    <t>invoicing</t>
+  </si>
+  <si>
+    <t>Fix1</t>
+  </si>
+  <si>
+    <t>Fixed value Variable</t>
+  </si>
+  <si>
+    <t>Var_FV_Demo1</t>
+  </si>
+  <si>
+    <t>IR Base Commissions Flat Rate Quota Based MTD</t>
+  </si>
+  <si>
+    <t>Lookup Table Variable</t>
+  </si>
+  <si>
+    <t>Var_LT_Demo4</t>
+  </si>
+  <si>
+    <t>MR Testrule</t>
+  </si>
+  <si>
+    <t>Aggregated Revenue against Territory based on Flat Rate</t>
+  </si>
+  <si>
+    <t>compensation plan</t>
+  </si>
+  <si>
+    <t>P_G_Demo1</t>
+  </si>
+  <si>
+    <t>R_T_Demo1</t>
+  </si>
+  <si>
+    <t>Var_RT_Demo2</t>
+  </si>
+  <si>
+    <t>Test RC</t>
+  </si>
+  <si>
+    <t>Territory_Demo</t>
+  </si>
+  <si>
+    <t>Var_T_Demo3</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -386,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,10 +516,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -410,13 +527,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -430,12 +547,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="52.7109375" customWidth="1"/>
+    <col min="13" max="20" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>